<commit_message>
Upgrade calamine and implement font size imports
</commit_message>
<xml_diff>
--- a/quadratic-core/test-files/styles.xlsx
+++ b/quadratic-core/test-files/styles.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70A6F88C-2E84-4BE2-9A98-31BA694825F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAD8560E-1984-4A53-A8B0-A74C532241FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Bold</t>
   </si>
@@ -58,6 +58,58 @@
   </si>
   <si>
     <t>This is a long line of text that will wrap.</t>
+  </si>
+  <si>
+    <t>Font Size Default</t>
+  </si>
+  <si>
+    <t>Font Size 14pt</t>
+  </si>
+  <si>
+    <t>Font Size 8pt</t>
+  </si>
+  <si>
+    <t>Font Size 36pt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>italic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://www.google.com</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -69,7 +121,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +166,47 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -158,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -180,6 +273,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -565,6 +664,31 @@
         <v>45859.548275462963</v>
       </c>
     </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18.75">
+      <c r="A16" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="92.25">
+      <c r="A18" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>